<commit_message>
lưu giá trị hourlyManhours vào firebase
</commit_message>
<xml_diff>
--- a/Quy trình.xlsx
+++ b/Quy trình.xlsx
@@ -2,15 +2,16 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
+  <workbookPr filterPrivacy="1"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Role" sheetId="1" r:id="rId1"/>
     <sheet name="QT" sheetId="2" r:id="rId2"/>
+    <sheet name="Task" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="152511"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -20,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="49">
   <si>
     <t>STT</t>
   </si>
@@ -170,11 +171,23 @@
   <si>
     <t>Áp dụng kế hoạch làm việc</t>
   </si>
+  <si>
+    <t>Taok giao diện mobile cho màn hình đăng ký của nhân viên</t>
+  </si>
+  <si>
+    <t>Thiết lập logic</t>
+  </si>
+  <si>
+    <t>Manhour</t>
+  </si>
+  <si>
+    <t>POS Manhour cần thiết (h) = Số lượng khách hàng * 1 (min)</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -268,6 +281,86 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>66675</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>47625</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>255780</xdr:colOff>
+      <xdr:row>34</xdr:row>
+      <xdr:rowOff>65887</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Picture 1"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="676275" y="238125"/>
+          <a:ext cx="11161905" cy="6304762"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>9525</xdr:colOff>
+      <xdr:row>36</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>21</xdr:col>
+      <xdr:colOff>142875</xdr:colOff>
+      <xdr:row>71</xdr:row>
+      <xdr:rowOff>175800</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="3" name="Picture 2"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill rotWithShape="1">
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2"/>
+        <a:srcRect r="13604"/>
+        <a:stretch/>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="619125" y="6858000"/>
+          <a:ext cx="12325350" cy="6843300"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -749,7 +842,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="G9" sqref="G9"/>
     </sheetView>
   </sheetViews>
@@ -868,4 +961,52 @@
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:X38"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
+      <selection activeCell="Y47" sqref="Y47"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1">
+        <v>1</v>
+      </c>
+      <c r="B1" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="36" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="A36">
+        <v>2</v>
+      </c>
+      <c r="B36" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="37" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="W37">
+        <v>1</v>
+      </c>
+      <c r="X37" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="38" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="W38">
+        <v>2</v>
+      </c>
+      <c r="X38" t="s">
+        <v>48</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>